<commit_message>
Fixing add and remove feature
</commit_message>
<xml_diff>
--- a/list-pegawai.xlsx
+++ b/list-pegawai.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\Python\PKL-Project2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E370F35-C3CB-4332-ACC4-75A7B3C29867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="4620" yWindow="1095" windowWidth="17505" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="67">
   <si>
     <t>Nama</t>
   </si>
@@ -194,13 +213,34 @@
   </si>
   <si>
     <t>'199311112013122001</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>CUTI</t>
+  </si>
+  <si>
+    <t>DL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,24 +292,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -307,7 +356,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -341,6 +390,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -375,9 +425,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -550,14 +601,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AH20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="25" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="32" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,8 +632,98 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1">
+        <v>11</v>
+      </c>
+      <c r="P1" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1">
+        <v>15</v>
+      </c>
+      <c r="T1" s="1">
+        <v>16</v>
+      </c>
+      <c r="U1" s="1">
+        <v>17</v>
+      </c>
+      <c r="V1" s="1">
+        <v>18</v>
+      </c>
+      <c r="W1" s="1">
+        <v>19</v>
+      </c>
+      <c r="X1" s="1">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>21</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>22</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>23</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>24</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>25</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>26</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>27</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>28</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>29</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -581,8 +736,98 @@
       <c r="D2" t="s">
         <v>41</v>
       </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" t="s">
+        <v>61</v>
+      </c>
+      <c r="T2" t="s">
+        <v>60</v>
+      </c>
+      <c r="U2" t="s">
+        <v>61</v>
+      </c>
+      <c r="V2" t="s">
+        <v>60</v>
+      </c>
+      <c r="W2" t="s">
+        <v>61</v>
+      </c>
+      <c r="X2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -595,8 +840,98 @@
       <c r="D3" t="s">
         <v>42</v>
       </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O3" t="s">
+        <v>63</v>
+      </c>
+      <c r="P3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R3" t="s">
+        <v>63</v>
+      </c>
+      <c r="S3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T3" t="s">
+        <v>62</v>
+      </c>
+      <c r="U3" t="s">
+        <v>62</v>
+      </c>
+      <c r="V3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -609,8 +944,98 @@
       <c r="D4" t="s">
         <v>43</v>
       </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M4" t="s">
+        <v>62</v>
+      </c>
+      <c r="N4" t="s">
+        <v>62</v>
+      </c>
+      <c r="O4" t="s">
+        <v>62</v>
+      </c>
+      <c r="P4" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>62</v>
+      </c>
+      <c r="R4" t="s">
+        <v>62</v>
+      </c>
+      <c r="S4" t="s">
+        <v>64</v>
+      </c>
+      <c r="T4" t="s">
+        <v>62</v>
+      </c>
+      <c r="U4" t="s">
+        <v>64</v>
+      </c>
+      <c r="V4" t="s">
+        <v>62</v>
+      </c>
+      <c r="W4" t="s">
+        <v>64</v>
+      </c>
+      <c r="X4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -623,8 +1048,98 @@
       <c r="D5" t="s">
         <v>44</v>
       </c>
+      <c r="E5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" t="s">
+        <v>62</v>
+      </c>
+      <c r="M5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N5" t="s">
+        <v>62</v>
+      </c>
+      <c r="O5" t="s">
+        <v>60</v>
+      </c>
+      <c r="P5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R5" t="s">
+        <v>64</v>
+      </c>
+      <c r="S5" t="s">
+        <v>62</v>
+      </c>
+      <c r="T5" t="s">
+        <v>60</v>
+      </c>
+      <c r="U5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V5" t="s">
+        <v>62</v>
+      </c>
+      <c r="W5" t="s">
+        <v>64</v>
+      </c>
+      <c r="X5" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -637,8 +1152,98 @@
       <c r="D6" t="s">
         <v>45</v>
       </c>
+      <c r="E6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" t="s">
+        <v>65</v>
+      </c>
+      <c r="J6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" t="s">
+        <v>65</v>
+      </c>
+      <c r="L6" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" t="s">
+        <v>60</v>
+      </c>
+      <c r="O6" t="s">
+        <v>61</v>
+      </c>
+      <c r="P6" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>61</v>
+      </c>
+      <c r="R6" t="s">
+        <v>62</v>
+      </c>
+      <c r="S6" t="s">
+        <v>60</v>
+      </c>
+      <c r="T6" t="s">
+        <v>61</v>
+      </c>
+      <c r="U6" t="s">
+        <v>62</v>
+      </c>
+      <c r="V6" t="s">
+        <v>62</v>
+      </c>
+      <c r="W6" t="s">
+        <v>64</v>
+      </c>
+      <c r="X6" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -651,8 +1256,98 @@
       <c r="D7" t="s">
         <v>46</v>
       </c>
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" t="s">
+        <v>64</v>
+      </c>
+      <c r="L7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" t="s">
+        <v>61</v>
+      </c>
+      <c r="O7" t="s">
+        <v>62</v>
+      </c>
+      <c r="P7" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>62</v>
+      </c>
+      <c r="R7" t="s">
+        <v>60</v>
+      </c>
+      <c r="S7" t="s">
+        <v>61</v>
+      </c>
+      <c r="T7" t="s">
+        <v>62</v>
+      </c>
+      <c r="U7" t="s">
+        <v>66</v>
+      </c>
+      <c r="V7" t="s">
+        <v>66</v>
+      </c>
+      <c r="W7" t="s">
+        <v>66</v>
+      </c>
+      <c r="X7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -665,8 +1360,98 @@
       <c r="D8" t="s">
         <v>47</v>
       </c>
+      <c r="E8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" t="s">
+        <v>62</v>
+      </c>
+      <c r="L8" t="s">
+        <v>62</v>
+      </c>
+      <c r="M8" t="s">
+        <v>62</v>
+      </c>
+      <c r="N8" t="s">
+        <v>62</v>
+      </c>
+      <c r="O8" t="s">
+        <v>62</v>
+      </c>
+      <c r="P8" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R8" t="s">
+        <v>62</v>
+      </c>
+      <c r="S8" t="s">
+        <v>62</v>
+      </c>
+      <c r="T8" t="s">
+        <v>62</v>
+      </c>
+      <c r="U8" t="s">
+        <v>62</v>
+      </c>
+      <c r="V8" t="s">
+        <v>62</v>
+      </c>
+      <c r="W8" t="s">
+        <v>62</v>
+      </c>
+      <c r="X8" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -679,8 +1464,98 @@
       <c r="D9" t="s">
         <v>48</v>
       </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" t="s">
+        <v>65</v>
+      </c>
+      <c r="L9" t="s">
+        <v>65</v>
+      </c>
+      <c r="M9" t="s">
+        <v>62</v>
+      </c>
+      <c r="N9" t="s">
+        <v>62</v>
+      </c>
+      <c r="O9" t="s">
+        <v>64</v>
+      </c>
+      <c r="P9" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>64</v>
+      </c>
+      <c r="R9" t="s">
+        <v>62</v>
+      </c>
+      <c r="S9" t="s">
+        <v>62</v>
+      </c>
+      <c r="T9" t="s">
+        <v>64</v>
+      </c>
+      <c r="U9" t="s">
+        <v>62</v>
+      </c>
+      <c r="V9" t="s">
+        <v>64</v>
+      </c>
+      <c r="W9" t="s">
+        <v>62</v>
+      </c>
+      <c r="X9" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -693,8 +1568,98 @@
       <c r="D10" t="s">
         <v>49</v>
       </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" t="s">
+        <v>62</v>
+      </c>
+      <c r="L10" t="s">
+        <v>60</v>
+      </c>
+      <c r="M10" t="s">
+        <v>61</v>
+      </c>
+      <c r="N10" t="s">
+        <v>62</v>
+      </c>
+      <c r="O10" t="s">
+        <v>64</v>
+      </c>
+      <c r="P10" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>62</v>
+      </c>
+      <c r="R10" t="s">
+        <v>66</v>
+      </c>
+      <c r="S10" t="s">
+        <v>66</v>
+      </c>
+      <c r="T10" t="s">
+        <v>66</v>
+      </c>
+      <c r="U10" t="s">
+        <v>66</v>
+      </c>
+      <c r="V10" t="s">
+        <v>66</v>
+      </c>
+      <c r="W10" t="s">
+        <v>66</v>
+      </c>
+      <c r="X10" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -707,8 +1672,98 @@
       <c r="D11" t="s">
         <v>50</v>
       </c>
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" t="s">
+        <v>62</v>
+      </c>
+      <c r="L11" t="s">
+        <v>62</v>
+      </c>
+      <c r="M11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N11" t="s">
+        <v>62</v>
+      </c>
+      <c r="O11" t="s">
+        <v>62</v>
+      </c>
+      <c r="P11" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>62</v>
+      </c>
+      <c r="R11" t="s">
+        <v>62</v>
+      </c>
+      <c r="S11" t="s">
+        <v>62</v>
+      </c>
+      <c r="T11" t="s">
+        <v>62</v>
+      </c>
+      <c r="U11" t="s">
+        <v>62</v>
+      </c>
+      <c r="V11" t="s">
+        <v>62</v>
+      </c>
+      <c r="W11" t="s">
+        <v>62</v>
+      </c>
+      <c r="X11" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -721,8 +1776,98 @@
       <c r="D12" t="s">
         <v>51</v>
       </c>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L12" t="s">
+        <v>60</v>
+      </c>
+      <c r="M12" t="s">
+        <v>61</v>
+      </c>
+      <c r="N12" t="s">
+        <v>62</v>
+      </c>
+      <c r="O12" t="s">
+        <v>64</v>
+      </c>
+      <c r="P12" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>60</v>
+      </c>
+      <c r="R12" t="s">
+        <v>61</v>
+      </c>
+      <c r="S12" t="s">
+        <v>62</v>
+      </c>
+      <c r="T12" t="s">
+        <v>64</v>
+      </c>
+      <c r="U12" t="s">
+        <v>62</v>
+      </c>
+      <c r="V12" t="s">
+        <v>64</v>
+      </c>
+      <c r="W12" t="s">
+        <v>62</v>
+      </c>
+      <c r="X12" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -735,8 +1880,98 @@
       <c r="D13" t="s">
         <v>52</v>
       </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" t="s">
+        <v>64</v>
+      </c>
+      <c r="I13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" t="s">
+        <v>64</v>
+      </c>
+      <c r="L13" t="s">
+        <v>62</v>
+      </c>
+      <c r="M13" t="s">
+        <v>64</v>
+      </c>
+      <c r="N13" t="s">
+        <v>62</v>
+      </c>
+      <c r="O13" t="s">
+        <v>62</v>
+      </c>
+      <c r="P13" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>62</v>
+      </c>
+      <c r="R13" t="s">
+        <v>60</v>
+      </c>
+      <c r="S13" t="s">
+        <v>61</v>
+      </c>
+      <c r="T13" t="s">
+        <v>62</v>
+      </c>
+      <c r="U13" t="s">
+        <v>64</v>
+      </c>
+      <c r="V13" t="s">
+        <v>60</v>
+      </c>
+      <c r="W13" t="s">
+        <v>61</v>
+      </c>
+      <c r="X13" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -749,8 +1984,98 @@
       <c r="D14" t="s">
         <v>53</v>
       </c>
+      <c r="E14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J14" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" t="s">
+        <v>62</v>
+      </c>
+      <c r="L14" t="s">
+        <v>64</v>
+      </c>
+      <c r="M14" t="s">
+        <v>62</v>
+      </c>
+      <c r="N14" t="s">
+        <v>62</v>
+      </c>
+      <c r="O14" t="s">
+        <v>60</v>
+      </c>
+      <c r="P14" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>62</v>
+      </c>
+      <c r="R14" t="s">
+        <v>64</v>
+      </c>
+      <c r="S14" t="s">
+        <v>64</v>
+      </c>
+      <c r="T14" t="s">
+        <v>62</v>
+      </c>
+      <c r="U14" t="s">
+        <v>62</v>
+      </c>
+      <c r="V14" t="s">
+        <v>62</v>
+      </c>
+      <c r="W14" t="s">
+        <v>60</v>
+      </c>
+      <c r="X14" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -763,8 +2088,98 @@
       <c r="D15" t="s">
         <v>54</v>
       </c>
+      <c r="E15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K15" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15" t="s">
+        <v>61</v>
+      </c>
+      <c r="M15" t="s">
+        <v>62</v>
+      </c>
+      <c r="N15" t="s">
+        <v>64</v>
+      </c>
+      <c r="O15" t="s">
+        <v>62</v>
+      </c>
+      <c r="P15" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>61</v>
+      </c>
+      <c r="R15" t="s">
+        <v>64</v>
+      </c>
+      <c r="S15" t="s">
+        <v>62</v>
+      </c>
+      <c r="T15" t="s">
+        <v>62</v>
+      </c>
+      <c r="U15" t="s">
+        <v>62</v>
+      </c>
+      <c r="V15" t="s">
+        <v>60</v>
+      </c>
+      <c r="W15" t="s">
+        <v>61</v>
+      </c>
+      <c r="X15" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -777,8 +2192,98 @@
       <c r="D16" t="s">
         <v>55</v>
       </c>
+      <c r="E16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" t="s">
+        <v>62</v>
+      </c>
+      <c r="H16" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" t="s">
+        <v>62</v>
+      </c>
+      <c r="K16" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" t="s">
+        <v>61</v>
+      </c>
+      <c r="M16" t="s">
+        <v>62</v>
+      </c>
+      <c r="N16" t="s">
+        <v>64</v>
+      </c>
+      <c r="O16" t="s">
+        <v>62</v>
+      </c>
+      <c r="P16" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>61</v>
+      </c>
+      <c r="R16" t="s">
+        <v>62</v>
+      </c>
+      <c r="S16" t="s">
+        <v>64</v>
+      </c>
+      <c r="T16" t="s">
+        <v>62</v>
+      </c>
+      <c r="U16" t="s">
+        <v>60</v>
+      </c>
+      <c r="V16" t="s">
+        <v>61</v>
+      </c>
+      <c r="W16" t="s">
+        <v>62</v>
+      </c>
+      <c r="X16" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -791,8 +2296,98 @@
       <c r="D17" t="s">
         <v>56</v>
       </c>
+      <c r="E17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K17" t="s">
+        <v>62</v>
+      </c>
+      <c r="L17" t="s">
+        <v>64</v>
+      </c>
+      <c r="M17" t="s">
+        <v>62</v>
+      </c>
+      <c r="N17" t="s">
+        <v>60</v>
+      </c>
+      <c r="O17" t="s">
+        <v>61</v>
+      </c>
+      <c r="P17" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>64</v>
+      </c>
+      <c r="R17" t="s">
+        <v>62</v>
+      </c>
+      <c r="S17" t="s">
+        <v>60</v>
+      </c>
+      <c r="T17" t="s">
+        <v>61</v>
+      </c>
+      <c r="U17" t="s">
+        <v>60</v>
+      </c>
+      <c r="V17" t="s">
+        <v>61</v>
+      </c>
+      <c r="W17" t="s">
+        <v>62</v>
+      </c>
+      <c r="X17" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -805,8 +2400,98 @@
       <c r="D18" t="s">
         <v>57</v>
       </c>
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" t="s">
+        <v>62</v>
+      </c>
+      <c r="J18" t="s">
+        <v>60</v>
+      </c>
+      <c r="K18" t="s">
+        <v>61</v>
+      </c>
+      <c r="L18" t="s">
+        <v>60</v>
+      </c>
+      <c r="M18" t="s">
+        <v>61</v>
+      </c>
+      <c r="N18" t="s">
+        <v>60</v>
+      </c>
+      <c r="O18" t="s">
+        <v>61</v>
+      </c>
+      <c r="P18" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>60</v>
+      </c>
+      <c r="R18" t="s">
+        <v>61</v>
+      </c>
+      <c r="S18" t="s">
+        <v>60</v>
+      </c>
+      <c r="T18" t="s">
+        <v>61</v>
+      </c>
+      <c r="U18" t="s">
+        <v>62</v>
+      </c>
+      <c r="V18" t="s">
+        <v>62</v>
+      </c>
+      <c r="W18" t="s">
+        <v>60</v>
+      </c>
+      <c r="X18" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -819,8 +2504,98 @@
       <c r="D19" t="s">
         <v>58</v>
       </c>
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" t="s">
+        <v>64</v>
+      </c>
+      <c r="J19" t="s">
+        <v>62</v>
+      </c>
+      <c r="K19" t="s">
+        <v>64</v>
+      </c>
+      <c r="L19" t="s">
+        <v>62</v>
+      </c>
+      <c r="M19" t="s">
+        <v>62</v>
+      </c>
+      <c r="N19" t="s">
+        <v>64</v>
+      </c>
+      <c r="O19" t="s">
+        <v>62</v>
+      </c>
+      <c r="P19" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>64</v>
+      </c>
+      <c r="R19" t="s">
+        <v>62</v>
+      </c>
+      <c r="S19" t="s">
+        <v>64</v>
+      </c>
+      <c r="T19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V19" t="s">
+        <v>64</v>
+      </c>
+      <c r="W19" t="s">
+        <v>62</v>
+      </c>
+      <c r="X19" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -832,6 +2607,96 @@
       </c>
       <c r="D20" t="s">
         <v>59</v>
+      </c>
+      <c r="E20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" t="s">
+        <v>63</v>
+      </c>
+      <c r="K20" t="s">
+        <v>63</v>
+      </c>
+      <c r="L20" t="s">
+        <v>65</v>
+      </c>
+      <c r="M20" t="s">
+        <v>62</v>
+      </c>
+      <c r="N20" t="s">
+        <v>62</v>
+      </c>
+      <c r="O20" t="s">
+        <v>63</v>
+      </c>
+      <c r="P20" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>63</v>
+      </c>
+      <c r="R20" t="s">
+        <v>63</v>
+      </c>
+      <c r="S20" t="s">
+        <v>65</v>
+      </c>
+      <c r="T20" t="s">
+        <v>62</v>
+      </c>
+      <c r="U20" t="s">
+        <v>62</v>
+      </c>
+      <c r="V20" t="s">
+        <v>63</v>
+      </c>
+      <c r="W20" t="s">
+        <v>65</v>
+      </c>
+      <c r="X20" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>